<commit_message>
Assignment 2 added Q1(a) YTM
</commit_message>
<xml_diff>
--- a/static/files/Excel Tutorial.xlsx
+++ b/static/files/Excel Tutorial.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bus-vc\Desktop\Eric\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Dong\Dropbox\Work\Gooder\PhD\Website\web1\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B13E62-1DE1-4994-AD34-B98003E4D01A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18756" windowHeight="8136" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NPV and IRR" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="YTM" sheetId="2" r:id="rId3"/>
     <sheet name="DCF" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -166,7 +167,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
@@ -677,20 +678,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -758,7 +759,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -845,7 +846,7 @@
         <v>126347.50976878197</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -853,7 +854,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -862,7 +863,7 @@
         <v>-394395.79712080187</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -871,7 +872,7 @@
         <v>4.5167513239157353E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="P15" s="2"/>
     </row>
   </sheetData>
@@ -882,19 +883,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -902,7 +903,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -910,7 +911,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -918,7 +919,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>2021</v>
       </c>
@@ -929,7 +930,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>6</v>
       </c>
@@ -943,7 +944,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>7</v>
       </c>
@@ -957,7 +958,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>8</v>
       </c>
@@ -971,7 +972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" s="9" t="s">
         <v>18</v>
       </c>
@@ -988,7 +989,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>9</v>
       </c>
@@ -1002,7 +1003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>10</v>
       </c>
@@ -1016,7 +1017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>12</v>
       </c>
@@ -1033,7 +1034,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" s="9" t="s">
         <v>13</v>
       </c>
@@ -1050,7 +1051,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C15" s="9" t="s">
         <v>17</v>
       </c>
@@ -1067,7 +1068,7 @@
         <v>6200</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="10" t="s">
         <v>14</v>
       </c>
@@ -1084,7 +1085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" s="9" t="s">
         <v>15</v>
       </c>
@@ -1101,7 +1102,7 @@
         <v>-2600</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>16</v>
       </c>
@@ -1118,7 +1119,7 @@
         <v>8800</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>2</v>
       </c>
@@ -1133,21 +1134,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1155,7 +1156,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1172,7 +1173,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1189,7 +1190,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1199,7 +1200,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1209,7 +1210,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1220,23 +1221,23 @@
       <c r="H6" s="2"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="4">
-        <f>B6*2</f>
+        <f>B6*B3</f>
         <v>7.4310215546310884E-2</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>0</v>
       </c>
@@ -1271,42 +1272,53 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10">
+        <f>-B5</f>
         <v>-900</v>
       </c>
       <c r="C10">
+        <f>$F$2</f>
         <v>25</v>
       </c>
       <c r="D10">
+        <f t="shared" ref="D10:K10" si="0">$F$2</f>
         <v>25</v>
       </c>
       <c r="E10">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="F10">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="G10">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="H10">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="I10">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="J10">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="K10">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="L10">
+        <f>B1+F2</f>
         <v>1025</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1318,7 +1330,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1329,74 +1341,74 @@
       <c r="H12" s="2"/>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H13" s="2"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H14" s="2"/>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H15" s="2"/>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H16" s="2"/>
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H17" s="2"/>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H18" s="2"/>
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H19" s="2"/>
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H20" s="2"/>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H21" s="2"/>
       <c r="I21" s="5"/>
     </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H22" s="2"/>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H32" s="2"/>
     </row>
   </sheetData>
@@ -1406,19 +1418,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -1450,7 +1462,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1482,7 +1494,7 @@
         <v>755.2527138374403</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1505,7 +1517,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1535,7 +1547,7 @@
         <v>67.972744245369626</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1565,7 +1577,7 @@
         <v>42.822828874582868</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1595,7 +1607,7 @@
         <v>2.9048181301440081</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1625,7 +1637,7 @@
         <v>2.3238545041152068</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>16</v>
       </c>
@@ -1655,7 +1667,7 @@
         <v>37.594156240323656</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1664,7 +1676,7 @@
         <v>558.54174985623706</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -1673,7 +1685,7 @@
         <v>424.82774186924161</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -1681,7 +1693,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1689,7 +1701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -1697,7 +1709,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>

</xml_diff>